<commit_message>
updated testcases- API-WOrk order
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4B46FF-A484-4167-9F1D-99E6A38D502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B188BF4A-80C9-48CE-BF5B-F39554CADD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="88">
   <si>
     <t>API Mode</t>
   </si>
@@ -289,6 +289,27 @@
   </si>
   <si>
     <t>Transfer Sales Invoice</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Automation5501-1 (Stock-Mfg-LotYesSerialYes)</t>
+  </si>
+  <si>
+    <t>Automation5501-2 (Mfg-LotYes)</t>
+  </si>
+  <si>
+    <t>Automation5501-3 (Kit)</t>
+  </si>
+  <si>
+    <t>Automation5501-4 (Service)</t>
+  </si>
+  <si>
+    <t>Automation5501-5 (Misc)</t>
   </si>
 </sst>
 </file>
@@ -635,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,11 +668,12 @@
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,13 +690,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -691,9 +716,12 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1867,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D019CD-FE6F-4CBE-BD43-E1AA757A2A0A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,11 +1907,12 @@
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1900,13 +1929,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1922,10 +1954,13 @@
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1937,10 +1972,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E477E4AB-7195-46E9-AE4C-74460C3E66C8}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H1" sqref="H1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,13 +1986,14 @@
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1980,28 +2016,31 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2023,29 +2062,32 @@
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="s">
+        <v>83</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>20</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2067,29 +2109,32 @@
       <c r="G3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>40</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2111,29 +2156,32 @@
       <c r="G4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H4">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>85</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>50</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4">
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>20</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>50</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2155,20 +2203,23 @@
       <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>80</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2190,16 +2241,19 @@
       <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6" t="b">
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2211,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DBB80D-3005-41F8-86F4-7517B0EFE4BC}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,13 +2279,14 @@
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2254,28 +2309,31 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2297,29 +2355,32 @@
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="s">
+        <v>83</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>20</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2341,29 +2402,32 @@
       <c r="G3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>40</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2385,29 +2449,32 @@
       <c r="G4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H4">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>85</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>50</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4">
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>20</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>50</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2429,20 +2496,23 @@
       <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>80</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2464,16 +2534,19 @@
       <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6" t="b">
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2560,7 +2633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF58CD5-46D2-4094-A4C4-64F9F4BD8F76}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>